<commit_message>
Add inf to big5_main.xlsx
</commit_message>
<xml_diff>
--- a/big5_for_crawler.xlsx
+++ b/big5_for_crawler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\Documents\GitHub\psyprediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D56909-DBDD-411F-A610-0DA1F89D86AC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F4960E-69FA-49A5-A2E0-412152DB5C03}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="149">
   <si>
     <t>owner_id</t>
   </si>
@@ -460,6 +460,18 @@
   </si>
   <si>
     <t>http://psytests.org/result?v=pfqLj-iuWwuwvNSdPRb9</t>
+  </si>
+  <si>
+    <t>https://vk.com/ekimovalex</t>
+  </si>
+  <si>
+    <t>http://psytests.org/result?v=pfqOCrZZApR3RIR6CYBZ</t>
+  </si>
+  <si>
+    <t>https://vk.com/id175676662</t>
+  </si>
+  <si>
+    <t>http://psytests.org/result?v=pfqKFHO9b-WOuhiwaByt</t>
   </si>
 </sst>
 </file>
@@ -805,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J55" sqref="J55"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2124,6 +2136,46 @@
         <v>12</v>
       </c>
       <c r="G64" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>202230988</v>
+      </c>
+      <c r="B65" t="s">
+        <v>145</v>
+      </c>
+      <c r="C65" t="s">
+        <v>146</v>
+      </c>
+      <c r="D65">
+        <v>30</v>
+      </c>
+      <c r="E65" t="s">
+        <v>12</v>
+      </c>
+      <c r="G65" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>175676662</v>
+      </c>
+      <c r="B66" t="s">
+        <v>147</v>
+      </c>
+      <c r="C66" t="s">
+        <v>148</v>
+      </c>
+      <c r="D66">
+        <v>24</v>
+      </c>
+      <c r="E66" t="s">
+        <v>9</v>
+      </c>
+      <c r="G66" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>